<commit_message>
lydata för zz033 tillagd
</commit_message>
<xml_diff>
--- a/Rawdata/lydata.xlsx
+++ b/Rawdata/lydata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="37">
   <si>
     <t>lya</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>zz033</t>
+  </si>
+  <si>
+    <t>91.5</t>
+  </si>
+  <si>
+    <t>250 SV</t>
   </si>
 </sst>
 </file>
@@ -483,9 +489,9 @@
   <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
+      <selection pane="bottomLeft" activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2345,50 +2351,380 @@
       <c r="A52" t="s">
         <v>34</v>
       </c>
+      <c r="B52">
+        <v>75</v>
+      </c>
+      <c r="C52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>-0.5</v>
+      </c>
+      <c r="F52">
+        <v>-0.6</v>
+      </c>
+      <c r="G52" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52">
+        <v>17</v>
+      </c>
+      <c r="I52" t="s">
+        <v>36</v>
+      </c>
+      <c r="J52">
+        <v>20</v>
+      </c>
+      <c r="K52">
+        <v>3</v>
+      </c>
+      <c r="L52" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>34</v>
       </c>
+      <c r="B53">
+        <v>75</v>
+      </c>
+      <c r="C53" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>-0.2</v>
+      </c>
+      <c r="F53">
+        <v>-0.3</v>
+      </c>
+      <c r="G53" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53">
+        <v>12</v>
+      </c>
+      <c r="I53" t="s">
+        <v>36</v>
+      </c>
+      <c r="J53">
+        <v>20</v>
+      </c>
+      <c r="K53">
+        <v>3</v>
+      </c>
+      <c r="L53" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>34</v>
       </c>
+      <c r="B54">
+        <v>75</v>
+      </c>
+      <c r="C54" t="s">
+        <v>35</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>3.8</v>
+      </c>
+      <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="G54" t="s">
+        <v>20</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54" t="s">
+        <v>36</v>
+      </c>
+      <c r="J54">
+        <v>20</v>
+      </c>
+      <c r="K54">
+        <v>3</v>
+      </c>
+      <c r="L54" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>34</v>
       </c>
+      <c r="B55">
+        <v>75</v>
+      </c>
+      <c r="C55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>-0.1</v>
+      </c>
+      <c r="F55">
+        <v>-0.2</v>
+      </c>
+      <c r="G55" t="s">
+        <v>13</v>
+      </c>
+      <c r="H55">
+        <v>8</v>
+      </c>
+      <c r="I55" t="s">
+        <v>36</v>
+      </c>
+      <c r="J55">
+        <v>20</v>
+      </c>
+      <c r="K55">
+        <v>3</v>
+      </c>
+      <c r="L55" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>34</v>
       </c>
+      <c r="B56">
+        <v>75</v>
+      </c>
+      <c r="C56" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>-0.2</v>
+      </c>
+      <c r="F56">
+        <v>-0.1</v>
+      </c>
+      <c r="G56" t="s">
+        <v>20</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>36</v>
+      </c>
+      <c r="J56">
+        <v>20</v>
+      </c>
+      <c r="K56">
+        <v>3</v>
+      </c>
+      <c r="L56" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>34</v>
       </c>
+      <c r="B57">
+        <v>75</v>
+      </c>
+      <c r="C57" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0.3</v>
+      </c>
+      <c r="F57">
+        <v>0.1</v>
+      </c>
+      <c r="G57" t="s">
+        <v>20</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>36</v>
+      </c>
+      <c r="J57">
+        <v>20</v>
+      </c>
+      <c r="K57">
+        <v>3</v>
+      </c>
+      <c r="L57" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>34</v>
       </c>
+      <c r="B58">
+        <v>75</v>
+      </c>
+      <c r="C58" t="s">
+        <v>35</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>-0.4</v>
+      </c>
+      <c r="F58">
+        <v>-0.5</v>
+      </c>
+      <c r="G58" t="s">
+        <v>13</v>
+      </c>
+      <c r="H58">
+        <v>22</v>
+      </c>
+      <c r="I58" t="s">
+        <v>36</v>
+      </c>
+      <c r="J58">
+        <v>20</v>
+      </c>
+      <c r="K58">
+        <v>3</v>
+      </c>
+      <c r="L58" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>34</v>
       </c>
+      <c r="B59">
+        <v>75</v>
+      </c>
+      <c r="C59" t="s">
+        <v>35</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>-0.3</v>
+      </c>
+      <c r="F59">
+        <v>-0.5</v>
+      </c>
+      <c r="G59" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59">
+        <v>5</v>
+      </c>
+      <c r="I59" t="s">
+        <v>36</v>
+      </c>
+      <c r="J59">
+        <v>20</v>
+      </c>
+      <c r="K59">
+        <v>3</v>
+      </c>
+      <c r="L59" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>34</v>
       </c>
+      <c r="B60">
+        <v>75</v>
+      </c>
+      <c r="C60" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>-0.2</v>
+      </c>
+      <c r="F60">
+        <v>-0.3</v>
+      </c>
+      <c r="G60" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60">
+        <v>3</v>
+      </c>
+      <c r="I60" t="s">
+        <v>36</v>
+      </c>
+      <c r="J60">
+        <v>20</v>
+      </c>
+      <c r="K60">
+        <v>3</v>
+      </c>
+      <c r="L60" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>34</v>
+      </c>
+      <c r="B61">
+        <v>75</v>
+      </c>
+      <c r="C61" t="s">
+        <v>35</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>-0.4</v>
+      </c>
+      <c r="F61">
+        <v>-0.4</v>
+      </c>
+      <c r="G61" t="s">
+        <v>20</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>36</v>
+      </c>
+      <c r="J61">
+        <v>20</v>
+      </c>
+      <c r="K61">
+        <v>3</v>
+      </c>
+      <c r="L61" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
014 och 096 klar
</commit_message>
<xml_diff>
--- a/Rawdata/lydata.xlsx
+++ b/Rawdata/lydata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="25440" windowHeight="14120" xr2:uid="{655D4D94-E2E7-4740-A411-42C071AC19FC}"/>
+    <workbookView xWindow="2800" yWindow="460" windowWidth="25440" windowHeight="14120" xr2:uid="{655D4D94-E2E7-4740-A411-42C071AC19FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="48">
   <si>
     <t>lya</t>
   </si>
@@ -150,6 +150,24 @@
   </si>
   <si>
     <t>Andra delen av lyan vid gps-punkten. Mäter snödjup där det är grävt fyra hål i snön av rävar. Rävarna verkar ha lämnat lyan. Ett färskt spår vid foderautomaten. Rävarna verkar också ha försökt gräva i marken ovanför foderautomaten nyligen.</t>
+  </si>
+  <si>
+    <t>zz014</t>
+  </si>
+  <si>
+    <t>130 SO</t>
+  </si>
+  <si>
+    <t>Om man räknar med nysnö är andel snöfri yta 70 %. Den snöfria ytan är då 236,6 kvadratmeter. Det fanns 11 hål på lyan men alla utom ett var täckt med snö. Jag borde ha undersökt om det bara var nysnö men det gjorde jag inte.</t>
+  </si>
+  <si>
+    <t>zz096</t>
+  </si>
+  <si>
+    <t>266 V</t>
+  </si>
+  <si>
+    <t>Lyan ligger i en sluttning med riktning 172 grader S. Dock skymmer en liten kulle lyan. Kullen har inga synliga öppningar och väldigt lite högt gräs. Lyans riktning blir snarare 266 grader. Vinkel svårt pga snö. Kullen framför lyan har en vinkel på 28 grader. Det är ett mycket färskt rävspår på lyan och ett grävt hål i snön bakom en sten 10 m norr om "kullen". Endast 1 synlig öppning som är igenisad. Andel snöfri yta är svårt att säga. Kullens snöfria area är 18,7 kvadratmeter men oklart om den är en del av lyan.</t>
   </si>
 </sst>
 </file>
@@ -501,12 +519,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF1A5DEB-CC56-1046-88D0-A286B21A1C04}">
-  <dimension ref="A1:M81"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C81" sqref="C81"/>
+      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3472,6 +3490,826 @@
         <v>41</v>
       </c>
     </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>42</v>
+      </c>
+      <c r="B82">
+        <v>90</v>
+      </c>
+      <c r="C82">
+        <v>449.5</v>
+      </c>
+      <c r="D82">
+        <v>1.2</v>
+      </c>
+      <c r="E82">
+        <v>0.9</v>
+      </c>
+      <c r="F82">
+        <v>0.5</v>
+      </c>
+      <c r="G82" t="s">
+        <v>20</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82" t="s">
+        <v>43</v>
+      </c>
+      <c r="J82">
+        <v>9</v>
+      </c>
+      <c r="K82">
+        <v>1</v>
+      </c>
+      <c r="L82" t="s">
+        <v>17</v>
+      </c>
+      <c r="M82" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>42</v>
+      </c>
+      <c r="B83">
+        <v>90</v>
+      </c>
+      <c r="C83">
+        <v>449.5</v>
+      </c>
+      <c r="D83">
+        <v>1.2</v>
+      </c>
+      <c r="E83">
+        <v>-0.1</v>
+      </c>
+      <c r="F83">
+        <v>0.1</v>
+      </c>
+      <c r="G83" t="s">
+        <v>13</v>
+      </c>
+      <c r="H83">
+        <v>5</v>
+      </c>
+      <c r="I83" t="s">
+        <v>43</v>
+      </c>
+      <c r="J83">
+        <v>9</v>
+      </c>
+      <c r="K83">
+        <v>1</v>
+      </c>
+      <c r="L83" t="s">
+        <v>17</v>
+      </c>
+      <c r="M83" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>42</v>
+      </c>
+      <c r="B84">
+        <v>90</v>
+      </c>
+      <c r="C84">
+        <v>449.5</v>
+      </c>
+      <c r="D84">
+        <v>1.2</v>
+      </c>
+      <c r="E84">
+        <v>-0.3</v>
+      </c>
+      <c r="F84">
+        <v>-0.4</v>
+      </c>
+      <c r="G84" t="s">
+        <v>12</v>
+      </c>
+      <c r="H84">
+        <v>12</v>
+      </c>
+      <c r="I84" t="s">
+        <v>43</v>
+      </c>
+      <c r="J84">
+        <v>9</v>
+      </c>
+      <c r="K84">
+        <v>1</v>
+      </c>
+      <c r="L84" t="s">
+        <v>17</v>
+      </c>
+      <c r="M84" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>42</v>
+      </c>
+      <c r="B85">
+        <v>90</v>
+      </c>
+      <c r="C85">
+        <v>449.5</v>
+      </c>
+      <c r="D85">
+        <v>1.2</v>
+      </c>
+      <c r="E85">
+        <v>-0.2</v>
+      </c>
+      <c r="F85">
+        <v>-0.3</v>
+      </c>
+      <c r="G85" t="s">
+        <v>13</v>
+      </c>
+      <c r="H85">
+        <v>12</v>
+      </c>
+      <c r="I85" t="s">
+        <v>43</v>
+      </c>
+      <c r="J85">
+        <v>9</v>
+      </c>
+      <c r="K85">
+        <v>1</v>
+      </c>
+      <c r="L85" t="s">
+        <v>17</v>
+      </c>
+      <c r="M85" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>42</v>
+      </c>
+      <c r="B86">
+        <v>90</v>
+      </c>
+      <c r="C86">
+        <v>449.5</v>
+      </c>
+      <c r="D86">
+        <v>1.2</v>
+      </c>
+      <c r="E86">
+        <v>-0.2</v>
+      </c>
+      <c r="F86">
+        <v>-0.4</v>
+      </c>
+      <c r="G86" t="s">
+        <v>20</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86" t="s">
+        <v>43</v>
+      </c>
+      <c r="J86">
+        <v>9</v>
+      </c>
+      <c r="K86">
+        <v>1</v>
+      </c>
+      <c r="L86" t="s">
+        <v>17</v>
+      </c>
+      <c r="M86" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>42</v>
+      </c>
+      <c r="B87">
+        <v>90</v>
+      </c>
+      <c r="C87">
+        <v>449.5</v>
+      </c>
+      <c r="D87">
+        <v>1.2</v>
+      </c>
+      <c r="E87">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F87">
+        <v>4.5</v>
+      </c>
+      <c r="G87" t="s">
+        <v>20</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+      <c r="I87" t="s">
+        <v>43</v>
+      </c>
+      <c r="J87">
+        <v>9</v>
+      </c>
+      <c r="K87">
+        <v>1</v>
+      </c>
+      <c r="L87" t="s">
+        <v>17</v>
+      </c>
+      <c r="M87" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>42</v>
+      </c>
+      <c r="B88">
+        <v>90</v>
+      </c>
+      <c r="C88">
+        <v>449.5</v>
+      </c>
+      <c r="D88">
+        <v>1.2</v>
+      </c>
+      <c r="E88">
+        <v>0.5</v>
+      </c>
+      <c r="F88">
+        <v>-0.3</v>
+      </c>
+      <c r="G88" t="s">
+        <v>20</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88" t="s">
+        <v>43</v>
+      </c>
+      <c r="J88">
+        <v>9</v>
+      </c>
+      <c r="K88">
+        <v>1</v>
+      </c>
+      <c r="L88" t="s">
+        <v>17</v>
+      </c>
+      <c r="M88" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>42</v>
+      </c>
+      <c r="B89">
+        <v>90</v>
+      </c>
+      <c r="C89">
+        <v>449.5</v>
+      </c>
+      <c r="D89">
+        <v>1.2</v>
+      </c>
+      <c r="E89">
+        <v>-0.3</v>
+      </c>
+      <c r="F89">
+        <v>-0.4</v>
+      </c>
+      <c r="G89" t="s">
+        <v>13</v>
+      </c>
+      <c r="H89">
+        <v>3</v>
+      </c>
+      <c r="I89" t="s">
+        <v>43</v>
+      </c>
+      <c r="J89">
+        <v>9</v>
+      </c>
+      <c r="K89">
+        <v>1</v>
+      </c>
+      <c r="L89" t="s">
+        <v>17</v>
+      </c>
+      <c r="M89" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>42</v>
+      </c>
+      <c r="B90">
+        <v>90</v>
+      </c>
+      <c r="C90">
+        <v>449.5</v>
+      </c>
+      <c r="D90">
+        <v>1.2</v>
+      </c>
+      <c r="E90">
+        <v>-0.3</v>
+      </c>
+      <c r="F90">
+        <v>-0.3</v>
+      </c>
+      <c r="G90" t="s">
+        <v>13</v>
+      </c>
+      <c r="H90">
+        <v>3</v>
+      </c>
+      <c r="I90" t="s">
+        <v>43</v>
+      </c>
+      <c r="J90">
+        <v>9</v>
+      </c>
+      <c r="K90">
+        <v>1</v>
+      </c>
+      <c r="L90" t="s">
+        <v>17</v>
+      </c>
+      <c r="M90" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>42</v>
+      </c>
+      <c r="B91">
+        <v>90</v>
+      </c>
+      <c r="C91">
+        <v>449.5</v>
+      </c>
+      <c r="D91">
+        <v>1.2</v>
+      </c>
+      <c r="E91">
+        <v>-0.3</v>
+      </c>
+      <c r="F91">
+        <v>-0.3</v>
+      </c>
+      <c r="G91" t="s">
+        <v>13</v>
+      </c>
+      <c r="H91">
+        <v>10</v>
+      </c>
+      <c r="I91" t="s">
+        <v>43</v>
+      </c>
+      <c r="J91">
+        <v>9</v>
+      </c>
+      <c r="K91">
+        <v>1</v>
+      </c>
+      <c r="L91" t="s">
+        <v>17</v>
+      </c>
+      <c r="M91" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>45</v>
+      </c>
+      <c r="B92">
+        <v>15</v>
+      </c>
+      <c r="C92">
+        <v>10.3</v>
+      </c>
+      <c r="D92">
+        <v>0.1</v>
+      </c>
+      <c r="E92">
+        <v>-0.3</v>
+      </c>
+      <c r="F92">
+        <v>-0.4</v>
+      </c>
+      <c r="G92" t="s">
+        <v>12</v>
+      </c>
+      <c r="H92">
+        <v>59</v>
+      </c>
+      <c r="I92" t="s">
+        <v>46</v>
+      </c>
+      <c r="J92">
+        <v>16</v>
+      </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
+      <c r="L92" t="s">
+        <v>23</v>
+      </c>
+      <c r="M92" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>45</v>
+      </c>
+      <c r="B93">
+        <v>15</v>
+      </c>
+      <c r="C93">
+        <v>10.3</v>
+      </c>
+      <c r="D93">
+        <v>0.1</v>
+      </c>
+      <c r="E93">
+        <v>-0.3</v>
+      </c>
+      <c r="F93">
+        <v>-0.4</v>
+      </c>
+      <c r="G93" t="s">
+        <v>12</v>
+      </c>
+      <c r="H93">
+        <v>16</v>
+      </c>
+      <c r="I93" t="s">
+        <v>46</v>
+      </c>
+      <c r="J93">
+        <v>16</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="L93" t="s">
+        <v>23</v>
+      </c>
+      <c r="M93" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>45</v>
+      </c>
+      <c r="B94">
+        <v>15</v>
+      </c>
+      <c r="C94">
+        <v>10.3</v>
+      </c>
+      <c r="D94">
+        <v>0.1</v>
+      </c>
+      <c r="E94">
+        <v>-0.3</v>
+      </c>
+      <c r="F94">
+        <v>-0.3</v>
+      </c>
+      <c r="G94" t="s">
+        <v>12</v>
+      </c>
+      <c r="H94">
+        <v>14</v>
+      </c>
+      <c r="I94" t="s">
+        <v>46</v>
+      </c>
+      <c r="J94">
+        <v>16</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+      <c r="L94" t="s">
+        <v>23</v>
+      </c>
+      <c r="M94" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>45</v>
+      </c>
+      <c r="B95">
+        <v>15</v>
+      </c>
+      <c r="C95">
+        <v>10.3</v>
+      </c>
+      <c r="D95">
+        <v>0.1</v>
+      </c>
+      <c r="E95">
+        <v>-0.5</v>
+      </c>
+      <c r="F95">
+        <v>-0.5</v>
+      </c>
+      <c r="G95" t="s">
+        <v>20</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95" t="s">
+        <v>46</v>
+      </c>
+      <c r="J95">
+        <v>16</v>
+      </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
+      <c r="L95" t="s">
+        <v>23</v>
+      </c>
+      <c r="M95" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>45</v>
+      </c>
+      <c r="B96">
+        <v>15</v>
+      </c>
+      <c r="C96">
+        <v>10.3</v>
+      </c>
+      <c r="D96">
+        <v>0.1</v>
+      </c>
+      <c r="E96">
+        <v>-0.4</v>
+      </c>
+      <c r="F96">
+        <v>-0.5</v>
+      </c>
+      <c r="G96" t="s">
+        <v>12</v>
+      </c>
+      <c r="H96">
+        <v>28</v>
+      </c>
+      <c r="I96" t="s">
+        <v>46</v>
+      </c>
+      <c r="J96">
+        <v>16</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="L96" t="s">
+        <v>23</v>
+      </c>
+      <c r="M96" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>45</v>
+      </c>
+      <c r="B97">
+        <v>15</v>
+      </c>
+      <c r="C97">
+        <v>10.3</v>
+      </c>
+      <c r="D97">
+        <v>0.1</v>
+      </c>
+      <c r="E97">
+        <v>-0.2</v>
+      </c>
+      <c r="F97">
+        <v>-0.3</v>
+      </c>
+      <c r="G97" t="s">
+        <v>20</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97" t="s">
+        <v>46</v>
+      </c>
+      <c r="J97">
+        <v>16</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97" t="s">
+        <v>23</v>
+      </c>
+      <c r="M97" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>45</v>
+      </c>
+      <c r="B98">
+        <v>15</v>
+      </c>
+      <c r="C98">
+        <v>10.3</v>
+      </c>
+      <c r="D98">
+        <v>0.1</v>
+      </c>
+      <c r="E98">
+        <v>-0.3</v>
+      </c>
+      <c r="F98">
+        <v>-0.4</v>
+      </c>
+      <c r="G98" t="s">
+        <v>20</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98" t="s">
+        <v>46</v>
+      </c>
+      <c r="J98">
+        <v>16</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98" t="s">
+        <v>23</v>
+      </c>
+      <c r="M98" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>45</v>
+      </c>
+      <c r="B99">
+        <v>15</v>
+      </c>
+      <c r="C99">
+        <v>10.3</v>
+      </c>
+      <c r="D99">
+        <v>0.1</v>
+      </c>
+      <c r="E99">
+        <v>-0.3</v>
+      </c>
+      <c r="F99">
+        <v>-0.4</v>
+      </c>
+      <c r="G99" t="s">
+        <v>20</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99" t="s">
+        <v>46</v>
+      </c>
+      <c r="J99">
+        <v>16</v>
+      </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99" t="s">
+        <v>23</v>
+      </c>
+      <c r="M99" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>45</v>
+      </c>
+      <c r="B100">
+        <v>15</v>
+      </c>
+      <c r="C100">
+        <v>10.3</v>
+      </c>
+      <c r="D100">
+        <v>0.1</v>
+      </c>
+      <c r="E100">
+        <v>-0.2</v>
+      </c>
+      <c r="F100">
+        <v>-0.3</v>
+      </c>
+      <c r="G100" t="s">
+        <v>20</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100" t="s">
+        <v>46</v>
+      </c>
+      <c r="J100">
+        <v>16</v>
+      </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
+      <c r="L100" t="s">
+        <v>23</v>
+      </c>
+      <c r="M100" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>45</v>
+      </c>
+      <c r="B101">
+        <v>15</v>
+      </c>
+      <c r="C101">
+        <v>10.3</v>
+      </c>
+      <c r="D101">
+        <v>0.1</v>
+      </c>
+      <c r="E101">
+        <v>-0.3</v>
+      </c>
+      <c r="F101">
+        <v>-0.4</v>
+      </c>
+      <c r="G101" t="s">
+        <v>12</v>
+      </c>
+      <c r="H101">
+        <v>29</v>
+      </c>
+      <c r="I101" t="s">
+        <v>46</v>
+      </c>
+      <c r="J101">
+        <v>16</v>
+      </c>
+      <c r="K101">
+        <v>0</v>
+      </c>
+      <c r="L101" t="s">
+        <v>23</v>
+      </c>
+      <c r="M101" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>

</xml_diff>